<commit_message>
Sheet to Object[][] in main methods
</commit_message>
<xml_diff>
--- a/test_data/orange_test_data.xlsx
+++ b/test_data/orange_test_data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -52,6 +52,72 @@
   </si>
   <si>
     <t>Expected Error</t>
+  </si>
+  <si>
+    <t>peter124</t>
+  </si>
+  <si>
+    <t>peter125</t>
+  </si>
+  <si>
+    <t>peter126</t>
+  </si>
+  <si>
+    <t>peter127</t>
+  </si>
+  <si>
+    <t>peter128</t>
+  </si>
+  <si>
+    <t>peter129</t>
+  </si>
+  <si>
+    <t>peter130</t>
+  </si>
+  <si>
+    <t>peter131</t>
+  </si>
+  <si>
+    <t>peter132</t>
+  </si>
+  <si>
+    <t>peter133</t>
+  </si>
+  <si>
+    <t>peter134</t>
+  </si>
+  <si>
+    <t>peter135</t>
+  </si>
+  <si>
+    <t>peter136</t>
+  </si>
+  <si>
+    <t>peter137</t>
+  </si>
+  <si>
+    <t>peter138</t>
+  </si>
+  <si>
+    <t>peter139</t>
+  </si>
+  <si>
+    <t>peter140</t>
+  </si>
+  <si>
+    <t>peter141</t>
+  </si>
+  <si>
+    <t>peter142</t>
+  </si>
+  <si>
+    <t>peter143</t>
+  </si>
+  <si>
+    <t>peter144</t>
+  </si>
+  <si>
+    <t>peter145</t>
   </si>
 </sst>
 </file>
@@ -381,10 +447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,6 +488,248 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>